<commit_message>
feat: include KEGG definitions for each level in dataframe and Excel file
</commit_message>
<xml_diff>
--- a/src/output_grouping_cho.xlsx
+++ b/src/output_grouping_cho.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:H150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,21 @@
           <t>Level_3</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Level_1 Function</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Level_2 Function</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Level_3 Function</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -486,6 +501,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -513,6 +543,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -540,6 +585,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -567,6 +627,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -594,6 +669,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -621,6 +711,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -648,6 +753,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -675,6 +795,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -702,6 +837,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -729,6 +879,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -756,6 +921,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -783,6 +963,21 @@
           <t>['09180', '09182', '03000']</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Transcription factors [BR:sce03000]</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -810,6 +1005,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -837,6 +1047,21 @@
           <t>['09100', '09102', '00190']</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Energy metabolism</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Oxidative phosphorylation</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -864,6 +1089,21 @@
           <t>['09180', '09182', '04131']</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Membrane trafficking [BR:sce04131]</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -891,6 +1131,21 @@
           <t>['09100', '09102', '00190']</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Energy metabolism</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Oxidative phosphorylation</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -918,6 +1173,21 @@
           <t>['09100', '09101', '00500']</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Carbohydrate metabolism</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Starch and sucrose metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -945,6 +1215,21 @@
           <t>['09100', '09108', '00130']</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Metabolism of cofactors and vitamins</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Ubiquinone and other terpenoid-quinone biosynthesis</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -972,6 +1257,21 @@
           <t>['09100', '09101', '00020']</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Carbohydrate metabolism</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Citrate cycle (TCA cycle)</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -999,6 +1299,21 @@
           <t>['09100', '09101', '00010']</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Carbohydrate metabolism</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Glycolysis / Gluconeogenesis</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1026,6 +1341,21 @@
           <t>['09100', '09102', '00190']</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Energy metabolism</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Oxidative phosphorylation</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1053,6 +1383,21 @@
           <t>['09100', '09103', '00061']</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Lipid metabolism</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Fatty acid biosynthesis</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1080,6 +1425,21 @@
           <t>['09180', '09182', '04131']</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Membrane trafficking [BR:sce04131]</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1107,6 +1467,21 @@
           <t>['09100', '09101', '00620']</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Carbohydrate metabolism</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Pyruvate metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1134,6 +1509,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1161,6 +1551,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1188,6 +1593,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1215,6 +1635,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1242,6 +1677,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1269,6 +1719,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1296,6 +1761,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1323,6 +1803,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1350,6 +1845,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1377,6 +1887,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1404,6 +1929,21 @@
           <t>['09180', '09183', '04812']</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Protein families: signaling and cellular processes</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Cytoskeleton proteins [BR:sce04812]</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1431,6 +1971,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1458,6 +2013,21 @@
           <t>['09140', '09142', '04814']</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Cell motility</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Motor proteins</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1485,6 +2055,21 @@
           <t>['09180', '09181', '01001']</t>
         </is>
       </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Protein families: metabolism</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Protein kinases [BR:sce01001]</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1512,6 +2097,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1539,6 +2139,21 @@
           <t>['09180', '09183', '04812']</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Protein families: signaling and cellular processes</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Cytoskeleton proteins [BR:sce04812]</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1566,6 +2181,21 @@
           <t>['09180', '09183', '04147']</t>
         </is>
       </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Protein families: signaling and cellular processes</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Exosome [BR:sce04147]</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1593,6 +2223,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1620,6 +2265,21 @@
           <t>['09100', '09101', '00520']</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Carbohydrate metabolism</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Amino sugar and nucleotide sugar metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1647,6 +2307,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1674,6 +2349,21 @@
           <t>['09100', '09107', '00510']</t>
         </is>
       </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Glycan biosynthesis and metabolism</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>N-Glycan biosynthesis</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1701,6 +2391,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1728,6 +2433,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1755,6 +2475,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1782,6 +2517,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1809,6 +2559,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1836,6 +2601,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1863,6 +2643,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1890,6 +2685,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1917,6 +2727,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1944,6 +2769,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1971,6 +2811,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1998,6 +2853,21 @@
           <t>['09100', '09104', '00230']</t>
         </is>
       </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Nucleotide metabolism</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Purine metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2025,6 +2895,21 @@
           <t>['09100', '09104', '00240']</t>
         </is>
       </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Nucleotide metabolism</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Pyrimidine metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2052,6 +2937,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2079,6 +2979,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2106,6 +3021,21 @@
           <t>['09100', '09104', '00240']</t>
         </is>
       </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Nucleotide metabolism</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Pyrimidine metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2133,6 +3063,21 @@
           <t>['09180', '09182', '03400']</t>
         </is>
       </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>DNA repair and recombination proteins [BR:sce03400]</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2160,6 +3105,21 @@
           <t>['09120', '09124', '03410']</t>
         </is>
       </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Base excision repair</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2187,6 +3147,21 @@
           <t>['09120', '09124', '03430']</t>
         </is>
       </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Mismatch repair</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2214,6 +3189,21 @@
           <t>['09120', '09124', '03430']</t>
         </is>
       </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Mismatch repair</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2241,6 +3231,21 @@
           <t>['09120', '09124', '03430']</t>
         </is>
       </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Mismatch repair</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2268,6 +3273,21 @@
           <t>['09180', '09182', '03400']</t>
         </is>
       </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>DNA repair and recombination proteins [BR:sce03400]</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2295,6 +3315,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2322,6 +3357,21 @@
           <t>['09120', '09124', '03440']</t>
         </is>
       </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Homologous recombination</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2349,6 +3399,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2376,6 +3441,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2403,6 +3483,21 @@
           <t>['09180', '09182', '03012']</t>
         </is>
       </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Translation factors [BR:sce03012]</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2430,6 +3525,21 @@
           <t>['09120', '09124', '03410']</t>
         </is>
       </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Base excision repair</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2457,6 +3567,21 @@
           <t>['09180', '09182', '03032']</t>
         </is>
       </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>DNA replication proteins [BR:sce03032]</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2484,6 +3609,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2511,6 +3651,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2538,6 +3693,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2565,6 +3735,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2592,6 +3777,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2619,6 +3819,21 @@
           <t>['09120', '09122', '00970']</t>
         </is>
       </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Translation</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Aminoacyl-tRNA biosynthesis</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2646,6 +3861,21 @@
           <t>['09100', '09103', '00062']</t>
         </is>
       </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Lipid metabolism</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Fatty acid elongation</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2673,6 +3903,21 @@
           <t>['09100', '09105', '00270']</t>
         </is>
       </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Amino acid metabolism</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Cysteine and methionine metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2700,6 +3945,21 @@
           <t>['09100', '09103', '00061']</t>
         </is>
       </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Lipid metabolism</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Fatty acid biosynthesis</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2727,6 +3987,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2754,6 +4029,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2781,6 +4071,21 @@
           <t>['09140', '09142', '04814']</t>
         </is>
       </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Cell motility</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Motor proteins</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2808,6 +4113,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2835,6 +4155,21 @@
           <t>['09140', '09142', '04814']</t>
         </is>
       </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Cell motility</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Motor proteins</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2862,6 +4197,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2889,6 +4239,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2916,6 +4281,21 @@
           <t>['09140', '09142', '04814']</t>
         </is>
       </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Cell motility</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Motor proteins</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2943,6 +4323,21 @@
           <t>['09140', '09141', '04145']</t>
         </is>
       </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Transport and catabolism</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Phagosome</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2970,6 +4365,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2997,6 +4407,21 @@
           <t>['09180', '09183', '04812']</t>
         </is>
       </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Protein families: signaling and cellular processes</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Cytoskeleton proteins [BR:sce04812]</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3024,6 +4449,21 @@
           <t>['09100', '09104', '00230']</t>
         </is>
       </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Nucleotide metabolism</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Purine metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3051,6 +4491,21 @@
           <t>['09120', '09124', '03030']</t>
         </is>
       </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>DNA replication</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3078,6 +4533,21 @@
           <t>['09120', '09126', '03082']</t>
         </is>
       </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Chromosome</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>ATP-dependent chromatin remodeling</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3105,6 +4575,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3132,6 +4617,21 @@
           <t>['09120', '09124', '03440']</t>
         </is>
       </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Homologous recombination</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3159,6 +4659,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3186,6 +4701,21 @@
           <t>['09180', '09182', '03000']</t>
         </is>
       </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Transcription factors [BR:sce03000]</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3213,6 +4743,21 @@
           <t>['09180', '09182', '03021']</t>
         </is>
       </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>Transcription machinery [BR:sce03021]</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3240,6 +4785,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3267,6 +4827,21 @@
           <t>['09180', '09182', '03032']</t>
         </is>
       </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>DNA replication proteins [BR:sce03032]</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3294,6 +4869,21 @@
           <t>['09180', '09182', '03021']</t>
         </is>
       </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>Transcription machinery [BR:sce03021]</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3321,6 +4911,21 @@
           <t>['09180', '09182', '03021']</t>
         </is>
       </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Transcription machinery [BR:sce03021]</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3348,6 +4953,21 @@
           <t>['09100', '09101', '00010']</t>
         </is>
       </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>Carbohydrate metabolism</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Glycolysis / Gluconeogenesis</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3375,6 +4995,21 @@
           <t>['09180', '09182', '03016']</t>
         </is>
       </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>Transfer RNA biogenesis [BR:sce03016]</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3402,6 +5037,21 @@
           <t>['09100', '09107', '00513']</t>
         </is>
       </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Glycan biosynthesis and metabolism</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>Various types of N-glycan biosynthesis</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3429,6 +5079,21 @@
           <t>['09100', '09101', '00051']</t>
         </is>
       </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>Carbohydrate metabolism</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>Fructose and mannose metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -3456,6 +5121,21 @@
           <t>['09100', '09107', '00515']</t>
         </is>
       </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>Glycan biosynthesis and metabolism</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Mannose type O-glycan biosynthesis</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -3483,6 +5163,21 @@
           <t>['09180', '09182', '04131']</t>
         </is>
       </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Membrane trafficking [BR:sce04131]</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -3510,6 +5205,21 @@
           <t>['09100', '09107', '00515']</t>
         </is>
       </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>Glycan biosynthesis and metabolism</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>Mannose type O-glycan biosynthesis</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -3537,6 +5247,21 @@
           <t>['09120', '09122', '00970']</t>
         </is>
       </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>Translation</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>Aminoacyl-tRNA biosynthesis</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -3564,6 +5289,21 @@
           <t>['09190', '09191', '99981']</t>
         </is>
       </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Not Included in Pathway or Brite</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>Unclassified: metabolism</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>Carbohydrate metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -3591,6 +5331,21 @@
           <t>['09130', '09132', '04392']</t>
         </is>
       </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>Hippo signaling pathway - multiple species</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -3618,6 +5373,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3645,6 +5415,21 @@
           <t>['09180', '09183', '04812']</t>
         </is>
       </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>Protein families: signaling and cellular processes</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>Cytoskeleton proteins [BR:sce04812]</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -3672,6 +5457,21 @@
           <t>['09180', '09182', '04131']</t>
         </is>
       </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>Membrane trafficking [BR:sce04131]</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -3699,6 +5499,21 @@
           <t>['09140', '09141', '04138']</t>
         </is>
       </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>Transport and catabolism</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Autophagy - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -3726,6 +5541,21 @@
           <t>['09100', '09101', '00520']</t>
         </is>
       </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>Carbohydrate metabolism</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>Amino sugar and nucleotide sugar metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -3753,6 +5583,21 @@
           <t>['09120', '09124', '03420']</t>
         </is>
       </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>Replication and repair</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Nucleotide excision repair</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -3780,6 +5625,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -3807,6 +5667,21 @@
           <t>['09180', '09183', '02000']</t>
         </is>
       </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>Protein families: signaling and cellular processes</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>Transporters [BR:sce02000]</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -3834,6 +5709,21 @@
           <t>['09100', '09101', '00500']</t>
         </is>
       </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>Carbohydrate metabolism</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>Starch and sucrose metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -3861,6 +5751,21 @@
           <t>['09180', '09181', '01006']</t>
         </is>
       </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>Protein families: metabolism</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>Prenyltransferases [BR:sce01006]</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -3888,6 +5793,21 @@
           <t>['09180', '09183', '02000']</t>
         </is>
       </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>Protein families: signaling and cellular processes</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>Transporters [BR:sce02000]</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3915,6 +5835,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3942,6 +5877,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -3969,6 +5919,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -3996,6 +5961,21 @@
           <t>['09120', '09123', '04120']</t>
         </is>
       </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>Folding, sorting and degradation</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>Ubiquitin mediated proteolysis</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -4023,6 +6003,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -4050,6 +6045,21 @@
           <t>['09130', '09132', '04392']</t>
         </is>
       </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>Hippo signaling pathway - multiple species</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -4077,6 +6087,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -4104,6 +6129,21 @@
           <t>['09140', '09142', '04814']</t>
         </is>
       </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>Cell motility</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>Motor proteins</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -4131,6 +6171,21 @@
           <t>['09180', '09183', '04812']</t>
         </is>
       </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>Protein families: signaling and cellular processes</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>Cytoskeleton proteins [BR:sce04812]</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -4158,6 +6213,21 @@
           <t>['09180', '09182', '03019']</t>
         </is>
       </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>Messenger RNA biogenesis [BR:sce03019]</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -4185,6 +6255,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -4212,6 +6297,21 @@
           <t>['09180', '09181', '01001']</t>
         </is>
       </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>Protein families: metabolism</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>Protein kinases [BR:sce01001]</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -4239,6 +6339,21 @@
           <t>['09120', '09121', '03022']</t>
         </is>
       </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Genetic Information Processing</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>Transcription</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>Basal transcription factors</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -4266,6 +6381,21 @@
           <t>['09100', '09108', '00760']</t>
         </is>
       </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>Metabolism of cofactors and vitamins</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>Nicotinate and nicotinamide metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -4293,6 +6423,21 @@
           <t>['09180', '09182', '03036']</t>
         </is>
       </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>Chromosome and associated proteins [BR:sce03036]</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -4320,6 +6465,21 @@
           <t>['09140', '09143', '04111']</t>
         </is>
       </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>Cell cycle - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -4347,6 +6507,21 @@
           <t>['09180', '09182', '03000']</t>
         </is>
       </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>Transcription factors [BR:sce03000]</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -4374,6 +6549,21 @@
           <t>['09130', '09132', '04011']</t>
         </is>
       </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Environmental Information Processing</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>Signal transduction</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>MAPK signaling pathway - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -4401,6 +6591,21 @@
           <t>['09180', '09182', '03019']</t>
         </is>
       </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>Messenger RNA biogenesis [BR:sce03019]</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -4428,6 +6633,21 @@
           <t>['09100', '09101', '00052']</t>
         </is>
       </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Metabolism</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>Carbohydrate metabolism</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>Galactose metabolism</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -4455,6 +6675,21 @@
           <t>['09140', '09143', '04113']</t>
         </is>
       </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Cellular Processes</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>Cell growth and death</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>Meiosis - yeast</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -4480,6 +6715,21 @@
       <c r="E150" t="inlineStr">
         <is>
           <t>['09180', '09182', '04131']</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Brite Hierarchies</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>Protein families: genetic information processing</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>Membrane trafficking [BR:sce04131]</t>
         </is>
       </c>
     </row>

</xml_diff>